<commit_message>
more test scripts for qcmi fwhm conversion problem
</commit_message>
<xml_diff>
--- a/BraTaDio/offset_data/QCMI-BSA-offset.xlsx
+++ b/BraTaDio/offset_data/QCMI-BSA-offset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Documents\00 School Files 00\University\Mechano Biology Research\BraTaDio\offset_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F13867-5B99-477B-BAB8-E9C29200A46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27980F20-C567-40B2-8FE1-6990B5807BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="18600" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13380" yWindow="4005" windowWidth="18600" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,12 +90,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -104,7 +119,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,94 +405,97 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>4961272.0199999996</v>
       </c>
       <c r="B2">
         <v>65.069999999999993</v>
       </c>
-      <c r="C2">
-        <v>0</v>
+      <c r="C2" s="1">
+        <v>14866726.869999999</v>
       </c>
       <c r="D2">
         <v>71.55</v>
       </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="E2" s="1">
+        <v>24774372.23</v>
       </c>
       <c r="F2">
         <v>107.92</v>
       </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="G2" s="1">
+        <v>34680641.270000003</v>
       </c>
       <c r="H2">
         <v>170.63</v>
       </c>
-      <c r="I2">
-        <v>0</v>
+      <c r="I2" s="1">
+        <v>44587621.439999998</v>
       </c>
       <c r="J2">
         <v>228.35</v>
       </c>
-      <c r="K2">
-        <v>0</v>
+      <c r="K2" s="1">
+        <v>54494404.460000001</v>
       </c>
       <c r="L2">
         <v>316.2</v>
       </c>
-      <c r="M2">
-        <v>0</v>
+      <c r="M2" s="1">
+        <v>64401754.57</v>
       </c>
       <c r="N2">
         <v>402.16</v>

</xml_diff>